<commit_message>
Przejście zarządzania schematami na nowe api
</commit_message>
<xml_diff>
--- a/doc/schemas_v2/Sprzedawca Działu Części – zaawansowany.xlsx
+++ b/doc/schemas_v2/Sprzedawca Działu Części – zaawansowany.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="APSY" sheetId="1" state="visible" r:id="rId2"/>
@@ -1232,7 +1232,7 @@
   </sheetPr>
   <dimension ref="A1:AMJ4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -2216,8 +2216,8 @@
   </sheetPr>
   <dimension ref="A1:G194"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>